<commit_message>
ch maquina con  generador de errores y sugerencias
</commit_message>
<xml_diff>
--- a/chmaquina/cronograma ch.xlsx
+++ b/chmaquina/cronograma ch.xlsx
@@ -653,33 +653,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -748,18 +721,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -775,6 +736,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -784,8 +748,44 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,76 +1082,76 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="37"/>
-    </row>
-    <row r="3" spans="2:19" s="43" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="48"/>
+    </row>
+    <row r="3" spans="2:19" s="30" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="2:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="C5" s="48"/>
-      <c r="D5" s="45" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="47"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="35"/>
     </row>
     <row r="6" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="1">
@@ -1204,510 +1204,510 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="19"/>
+      <c r="D7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="10"/>
     </row>
     <row r="8" spans="2:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="23"/>
+      <c r="D8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="14"/>
     </row>
     <row r="9" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="23"/>
-    </row>
-    <row r="10" spans="2:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="14" t="s">
+      <c r="D9" s="15"/>
+      <c r="E9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="14"/>
+    </row>
+    <row r="10" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="37"/>
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="23"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="14"/>
     </row>
     <row r="11" spans="2:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="23"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="14"/>
     </row>
     <row r="12" spans="2:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="28"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="19"/>
     </row>
     <row r="13" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="10"/>
     </row>
     <row r="14" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="23"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="14"/>
     </row>
     <row r="15" spans="2:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="23"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="14"/>
     </row>
     <row r="16" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="23"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="14"/>
     </row>
     <row r="17" spans="2:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="15" t="s">
+      <c r="B17" s="41"/>
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="28"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="19"/>
     </row>
     <row r="18" spans="2:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="M18" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="34"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="25"/>
     </row>
     <row r="19" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="43"/>
+      <c r="C19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="M19" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N19" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="O19" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="23"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="14"/>
     </row>
     <row r="20" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="14" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N20" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="O20" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="P20" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="23"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="P20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="14"/>
     </row>
     <row r="21" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="14" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="M21" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N21" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="O21" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="P21" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="R21" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="S21" s="23"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="S21" s="14"/>
     </row>
     <row r="22" spans="2:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="14" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="R22" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="S22" s="23"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="S22" s="14"/>
     </row>
     <row r="23" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="14" t="s">
+      <c r="B23" s="43"/>
+      <c r="C23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="R23" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="S23" s="23"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="R23" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="S23" s="14"/>
     </row>
     <row r="24" spans="2:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="11"/>
-      <c r="C24" s="15" t="s">
+      <c r="B24" s="44"/>
+      <c r="C24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="28" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="19" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>